<commit_message>
misc updates preparing to send for revision
</commit_message>
<xml_diff>
--- a/figures/source/walden-I-prolation-canon.xlsx
+++ b/figures/source/walden-I-prolation-canon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="17580" windowHeight="18400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>flute</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>oboe</t>
+  </si>
+  <si>
+    <t>B/c</t>
+  </si>
+  <si>
+    <t>B/a</t>
   </si>
 </sst>
 </file>
@@ -253,9 +259,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.147455723093264"/>
+          <c:x val="0.11844355255064"/>
           <c:y val="0.122379035798964"/>
-          <c:w val="0.685890419947506"/>
+          <c:w val="0.820109515205072"/>
           <c:h val="0.753696103972133"/>
         </c:manualLayout>
       </c:layout>
@@ -494,11 +500,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124649464"/>
-        <c:axId val="2124642808"/>
+        <c:axId val="2105138472"/>
+        <c:axId val="2105145320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2124649464"/>
+        <c:axId val="2105138472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +521,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Motive Number</a:t>
+                  <a:t>SegmentNumber</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -526,7 +532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124642808"/>
+        <c:crossAx val="2105145320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -534,7 +540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124642808"/>
+        <c:axId val="2105145320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,7 +558,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Duration of motive (in quarter notes)</a:t>
+                  <a:t>Duration of segment (in quarter notes)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -564,21 +570,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124649464"/>
+        <c:crossAx val="2105138472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
@@ -645,9 +641,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.0955152990270869"/>
-          <c:y val="0.15049504950495"/>
+          <c:y val="0.120644259019861"/>
           <c:w val="0.741434348576832"/>
-          <c:h val="0.694719471947195"/>
+          <c:h val="0.757406040662827"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -662,7 +658,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>flute</c:v>
+                  <c:v>B/c</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -736,7 +732,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>oboe</c:v>
+                  <c:v>B/a</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -810,7 +806,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>clarinet</c:v>
+                  <c:v>B/c</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -885,11 +881,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125713288"/>
-        <c:axId val="2125707864"/>
+        <c:axId val="2139666856"/>
+        <c:axId val="2139672312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125713288"/>
+        <c:axId val="2139666856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +902,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Motive  Number</a:t>
+                  <a:t>Segment Number</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -917,7 +913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125707864"/>
+        <c:crossAx val="2139672312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,37 +921,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125707864"/>
+        <c:axId val="2139672312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Duration of motive (in quarter notes)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125713288"/>
+        <c:crossAx val="2139666856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,61 +977,60 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>187694</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11534140" y="215900"/>
+          <a:ext cx="9745980" cy="4254500"/>
+          <a:chOff x="11531600" y="215900"/>
+          <a:chExt cx="9767794" cy="4254500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Chart 1"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="11531600" y="215900"/>
+          <a:ext cx="4559322" cy="4254500"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Chart 2"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="15889194" y="215900"/>
+          <a:ext cx="5410200" cy="4254500"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1384,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1875,13 +1851,13 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2400,6 +2376,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="3" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
new figures and edits
</commit_message>
<xml_diff>
--- a/figures/source/walden-I-prolation-canon.xlsx
+++ b/figures/source/walden-I-prolation-canon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>flute</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>oboe</t>
-  </si>
-  <si>
-    <t>B/c</t>
   </si>
   <si>
     <t>B/a</t>
@@ -500,11 +497,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105138472"/>
-        <c:axId val="2105145320"/>
+        <c:axId val="-2121134024"/>
+        <c:axId val="-2128219192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2105138472"/>
+        <c:axId val="-2121134024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +518,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>SegmentNumber</a:t>
+                  <a:t>Segment Number</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -532,7 +529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105145320"/>
+        <c:crossAx val="-2128219192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -540,7 +537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105145320"/>
+        <c:axId val="-2128219192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -570,7 +567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105138472"/>
+        <c:crossAx val="-2121134024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -642,7 +639,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.0955152990270869"/>
           <c:y val="0.120644259019861"/>
-          <c:w val="0.741434348576832"/>
+          <c:w val="0.832477615011726"/>
           <c:h val="0.757406040662827"/>
         </c:manualLayout>
       </c:layout>
@@ -658,7 +655,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B/c</c:v>
+                  <c:v>B/a</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -806,7 +803,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B/c</c:v>
+                  <c:v>B/a</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -881,11 +878,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2139666856"/>
-        <c:axId val="2139672312"/>
+        <c:axId val="-2121289672"/>
+        <c:axId val="-2121714936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2139666856"/>
+        <c:axId val="-2121289672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +910,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139672312"/>
+        <c:crossAx val="-2121714936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -921,7 +918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2139672312"/>
+        <c:axId val="-2121714936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -932,7 +929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139666856"/>
+        <c:crossAx val="-2121289672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -943,11 +940,6 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
@@ -982,8 +974,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>66040</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>487681</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -995,9 +987,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="11534140" y="215900"/>
-          <a:ext cx="9745980" cy="4254500"/>
+          <a:ext cx="9090661" cy="4254500"/>
           <a:chOff x="11531600" y="215900"/>
-          <a:chExt cx="9767794" cy="4254500"/>
+          <a:chExt cx="9111008" cy="4254500"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:graphicFrame macro="">
@@ -1022,7 +1014,7 @@
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
           <a:off x="15889194" y="215900"/>
-          <a:ext cx="5410200" cy="4254500"/>
+          <a:ext cx="4753414" cy="4254500"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1361,7 +1353,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1854,7 +1846,7 @@
         <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24" t="s">
         <v>10</v>
@@ -2376,7 +2368,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="3" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>